<commit_message>
Add ExcelDataReader With Test Case
</commit_message>
<xml_diff>
--- a/UserInterface/ExcelData/ExampleData.xlsx
+++ b/UserInterface/ExcelData/ExampleData.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Skydiving</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>123</t>
+  </si>
+  <si>
+    <t>1,20,000</t>
   </si>
 </sst>
 </file>
@@ -507,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -845,15 +848,15 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>12387</v>
+      <c r="D1" t="s">
+        <v>28</v>
       </c>
       <c r="E1">
         <v>12.3215</v>
       </c>
       <c r="F1">
         <f>SUM(B1:D1)</f>
-        <v>13097</v>
+        <v>710</v>
       </c>
       <c r="G1">
         <v>98721</v>

</xml_diff>